<commit_message>
New Project to Push
</commit_message>
<xml_diff>
--- a/InputFile/Create_Work_Order.xlsx
+++ b/InputFile/Create_Work_Order.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asset_Management_Smoke_Test\Smoke_Test_Scenarios\InputFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DD35F5-5D9F-45DD-A90E-833FCE0847CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{0CB924B1-F626-438C-8648-1100A5928F47}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5B5096FC-3196-4F89-9EC8-FB58AA9D969C}"/>
+    <workbookView activeTab="6" firstSheet="2" windowHeight="11040" windowWidth="20730" xWindow="-120" xr2:uid="{5B5096FC-3196-4F89-9EC8-FB58AA9D969C}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="CWO_All_Field" sheetId="2" r:id="rId1"/>
+    <sheet name="CWO_Reverse" r:id="rId1" sheetId="2"/>
+    <sheet name="CWO_Exist_Reserve" r:id="rId2" sheetId="4"/>
+    <sheet name="Order_Status" r:id="rId3" sheetId="5"/>
+    <sheet name="Time_Sheet" r:id="rId4" sheetId="6"/>
+    <sheet name="Time_Sheet_Summary" r:id="rId5" sheetId="7"/>
+    <sheet name="Time_Sheet_Operation" r:id="rId6" sheetId="8"/>
+    <sheet name="CWO_PR" r:id="rId7" sheetId="3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="150">
   <si>
     <t>Field Type</t>
   </si>
@@ -101,9 +107,6 @@
     <t>Attach</t>
   </si>
   <si>
-    <t>DropDown</t>
-  </si>
-  <si>
     <t>Order Type</t>
   </si>
   <si>
@@ -161,9 +164,6 @@
     <t>Convert</t>
   </si>
   <si>
-    <t>ConvertButton</t>
-  </si>
-  <si>
     <t>FragmentButton</t>
   </si>
   <si>
@@ -185,9 +185,6 @@
     <t>Notification Number</t>
   </si>
   <si>
-    <t>10046625</t>
-  </si>
-  <si>
     <t>D-MOB-PAPB-CDU-001 Crude Oil Distillation Unit</t>
   </si>
   <si>
@@ -222,12 +219,286 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>50066048</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>50066049</t>
+  </si>
+  <si>
+    <t>N Stock item</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Field Value</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Reference No</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Latitude / Longitude</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>Break Down - D-MOB-PAPB-CDU-001 Crude Oi</t>
+  </si>
+  <si>
+    <t>VL01</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>General Data</t>
+  </si>
+  <si>
+    <t>Reservation</t>
+  </si>
+  <si>
+    <t>AttachDisplay</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>EXPORT.XLS</t>
+  </si>
+  <si>
+    <t>GetTexBoxValue</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>TableDisplay</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Storage Location</t>
+  </si>
+  <si>
+    <t>UoM</t>
+  </si>
+  <si>
+    <t>Available Qty</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>Aluminium coil wire</t>
+  </si>
+  <si>
+    <t>VS1</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Button_Disable</t>
+  </si>
+  <si>
+    <t>Time Entry</t>
+  </si>
+  <si>
+    <t>Time Sheet</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>D-MOB-PAPB-DHU-001 iee</t>
+  </si>
+  <si>
+    <t>10017208 Feed Exchanger</t>
+  </si>
+  <si>
+    <t>Monroe Twp, Pennsylvania</t>
+  </si>
+  <si>
+    <t>41.628 / -76.473</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>GetValue</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>TablePost</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>05:46:57</t>
+  </si>
+  <si>
+    <t>06:46:57</t>
+  </si>
+  <si>
+    <t>System Status</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>03.10.2023</t>
+  </si>
+  <si>
+    <t>Confirm No</t>
+  </si>
+  <si>
+    <t>Person Name</t>
+  </si>
+  <si>
+    <t>A Alexander</t>
+  </si>
+  <si>
+    <t>03-10-2023</t>
+  </si>
+  <si>
+    <t>Finish Time</t>
+  </si>
+  <si>
+    <t>Finish Date</t>
+  </si>
+  <si>
+    <t>Actual Hours</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>Final Conf.</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Final Confirmed</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>10046703</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>940526</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>541055</t>
+  </si>
+  <si>
+    <t>940519</t>
+  </si>
+  <si>
+    <t>Confirm No:449450</t>
+  </si>
+  <si>
+    <t>Partially Confirmed</t>
+  </si>
+  <si>
+    <t>10:14:40</t>
+  </si>
+  <si>
+    <t>03-21-2023</t>
+  </si>
+  <si>
+    <t>10:15:17</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10046704</t>
+  </si>
+  <si>
+    <t>940527</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>2.000</t>
+  </si>
+  <si>
+    <t>541056</t>
+  </si>
+  <si>
+    <t>Released</t>
+  </si>
+  <si>
+    <t>Confirm No:449458</t>
+  </si>
+  <si>
+    <t>11:47:16</t>
+  </si>
+  <si>
+    <t>11:47:52</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -277,27 +548,31 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="8">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="21" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -314,10 +589,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -352,7 +627,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -404,7 +679,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -515,21 +790,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -546,7 +821,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -598,27 +873,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme 2013 - 2022" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4094A1EE-E78A-471D-980D-6352D5DA882F}">
-  <dimension ref="A1:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4094A1EE-E78A-471D-980D-6352D5DA882F}">
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="57.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="41" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="57.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -629,38 +904,38 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -668,13 +943,1530 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>42</v>
       </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C31" xr:uid="{71D5513A-682A-44EA-8DE2-A2932C2CFBAA}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0E6601-2B9C-4C39-B640-7D64BA505113}">
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="57.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A65A451-82D7-40AA-9BF6-E830EF9EC3C2}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE2EBF2-E662-4694-BF56-450AB4C827D0}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9313D95E-3707-4841-A132-D92429A4DE83}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6D85ED-B63C-497E-9EDC-205396A9A97D}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F82414E-91B7-4967-A049-2333A658DA9C}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="57.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -682,7 +2474,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
@@ -690,288 +2482,266 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
+        <v>28</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="2">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="2">
-        <v>50066048</v>
+        <v>33</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="3">
-        <v>10</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>16</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="5"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C31" r:id="rId1" xr:uid="{71D5513A-682A-44EA-8DE2-A2932C2CFBAA}"/>
+    <hyperlink r:id="rId1" ref="C29" xr:uid="{69CE795E-7D20-4FBF-A5F8-2F3F716D5A71}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>